<commit_message>
Api restaurada con google sheet
</commit_message>
<xml_diff>
--- a/Data/guest.xlsx
+++ b/Data/guest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unmsmmail-my.sharepoint.com/personal/angel_ramirez_unmsm_edu_pe/Documents/Documentos/PersonalProjects/Wedding_Card/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\suiza\OneDrive\Documentos\Wedding_web\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="69" documentId="11_1DF9178A5BA0D468DFF93E11595ED87656CCAE51" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C706DDBB-A270-4629-99C8-0B9C174B8AAD}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1BE2BC0-6B40-4593-AB26-0429F32F6589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>ID</t>
   </si>
@@ -46,19 +46,43 @@
     <t>CONFIRMADO</t>
   </si>
   <si>
-    <t>D175KM</t>
-  </si>
-  <si>
     <t>F</t>
   </si>
   <si>
-    <t>FAMILIA PRINCIPAL :</t>
-  </si>
-  <si>
-    <t>EN ESPECIAL A USTEDES, QUE HAN HECHO ESTO POSIBLE, LOS AMAMOS Y ESPERAMOS EN ESTE DÍA.</t>
-  </si>
-  <si>
-    <t>QUERIDA MAMÁ Y PAPÁ</t>
+    <t>AMIGO01</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>PEREZ</t>
+  </si>
+  <si>
+    <t>JUAN</t>
+  </si>
+  <si>
+    <t>Nos vemos en la pista de baile</t>
+  </si>
+  <si>
+    <t>FAMILIA02</t>
+  </si>
+  <si>
+    <t>GOMEZ</t>
+  </si>
+  <si>
+    <t>MARIA</t>
+  </si>
+  <si>
+    <t>¡Felicidades! Ahí estaremos.</t>
+  </si>
+  <si>
+    <t>TIOPEPE</t>
+  </si>
+  <si>
+    <t>RAMIREZ</t>
+  </si>
+  <si>
+    <t>JOSÉ</t>
   </si>
 </sst>
 </file>
@@ -438,23 +462,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="241.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="241.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -480,36 +504,82 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>
       </c>
       <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <v>987654321</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3">
         <v>4</v>
       </c>
-      <c r="F2">
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <v>912345678</v>
+      </c>
+      <c r="H3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4">
         <v>1</v>
       </c>
-      <c r="G2">
-        <v>999999999</v>
-      </c>
-      <c r="H2" t="s">
-        <v>11</v>
+      <c r="F4">
+        <v>10</v>
       </c>
     </row>
-    <row r="39" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="47" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="50" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="51" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>